<commit_message>
Graphs made, slides prepared
</commit_message>
<xml_diff>
--- a/_NCSA Time sheet.xlsx
+++ b/_NCSA Time sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/snehgajiwala/Desktop/NCSA_genomics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A86ED1DF-2FA0-9A4A-BDEF-D97052365349}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB785CC1-C152-7844-B7E5-EE5F0D95E55F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16460" xr2:uid="{AD204971-E0E7-594B-AE4B-D8231DE2D531}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="31">
   <si>
     <t>Monday</t>
   </si>
@@ -111,16 +111,19 @@
     <t>9:00 to 16:00 =&gt;  Studying the 'forecast' and 'zoo' library; implementing solution from 'forecast' for missing values on CGM data</t>
   </si>
   <si>
-    <t>9:00 to 16:00 =&gt;  implementing solution from 'zoo' for missing values on CGM data</t>
-  </si>
-  <si>
-    <t>10:00 to 18:00 =&gt; Meeting with Justina; Implementing different solutions with CMG data; Reworking some old clustering plots</t>
-  </si>
-  <si>
-    <t>9:00 to 15:00 =&gt;  studying and implementing the 'mice' library</t>
-  </si>
-  <si>
-    <t>13:30 to 17:30 =&gt; summary plots for implemented solutions</t>
+    <t>10:00 to 18:00 =&gt; Meeting with Justina; Implementing different solutions with CMG data from library: zoo; Reworking some old clustering plots</t>
+  </si>
+  <si>
+    <t>13:30 to 17:30 =&gt; Implementing solutions from library: forecast</t>
+  </si>
+  <si>
+    <t>9:00 to 13:00 =&gt; Plotting error metrics for all; Preparing plots and slide decks for the meeting</t>
+  </si>
+  <si>
+    <t>9:00 to 16:00 =&gt;  Implementing solution from 'zoo' for missing values on CGM data</t>
+  </si>
+  <si>
+    <t>9:00 to 15:00 =&gt;  Studying and implementing the 'mice' library</t>
   </si>
 </sst>
 </file>
@@ -231,11 +234,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -554,7 +557,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22F60381-B2D6-6E48-8C0F-6899A86E0E4E}">
   <dimension ref="A2:K77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C70" sqref="C70"/>
     </sheetView>
   </sheetViews>
@@ -1018,7 +1021,7 @@
       <c r="B32" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C32" s="12" t="s">
+      <c r="C32" s="13" t="s">
         <v>14</v>
       </c>
       <c r="D32" s="10"/>
@@ -1031,7 +1034,7 @@
       <c r="B33" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C33" s="12"/>
+      <c r="C33" s="13"/>
       <c r="D33" s="10"/>
       <c r="E33" s="10"/>
     </row>
@@ -1042,7 +1045,7 @@
       <c r="B34" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C34" s="12"/>
+      <c r="C34" s="13"/>
     </row>
     <row r="35" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
@@ -1051,7 +1054,7 @@
       <c r="B35" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C35" s="12"/>
+      <c r="C35" s="13"/>
     </row>
     <row r="36" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
@@ -1060,7 +1063,7 @@
       <c r="B36" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C36" s="12"/>
+      <c r="C36" s="13"/>
     </row>
     <row r="37" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
@@ -1069,7 +1072,7 @@
       <c r="B37" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C37" s="12"/>
+      <c r="C37" s="13"/>
     </row>
     <row r="38" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
@@ -1078,7 +1081,7 @@
       <c r="B38" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C38" s="12"/>
+      <c r="C38" s="13"/>
     </row>
     <row r="39" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
@@ -1087,7 +1090,7 @@
       <c r="B39" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C39" s="12"/>
+      <c r="C39" s="13"/>
     </row>
     <row r="40" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
@@ -1096,7 +1099,7 @@
       <c r="B40" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C40" s="12"/>
+      <c r="C40" s="13"/>
     </row>
     <row r="41" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
@@ -1105,7 +1108,7 @@
       <c r="B41" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C41" s="12"/>
+      <c r="C41" s="13"/>
     </row>
     <row r="42" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
@@ -1114,7 +1117,7 @@
       <c r="B42" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C42" s="12"/>
+      <c r="C42" s="13"/>
     </row>
     <row r="43" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
@@ -1123,7 +1126,7 @@
       <c r="B43" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C43" s="12"/>
+      <c r="C43" s="13"/>
       <c r="F43" s="1">
         <f>SUM(E30:E41)</f>
         <v>9</v>
@@ -1152,7 +1155,7 @@
       <c r="B44" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C44" s="12"/>
+      <c r="C44" s="13"/>
     </row>
     <row r="45" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
@@ -1161,7 +1164,7 @@
       <c r="B45" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C45" s="12"/>
+      <c r="C45" s="13"/>
     </row>
     <row r="46" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
@@ -1170,7 +1173,7 @@
       <c r="B46" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C46" s="12"/>
+      <c r="C46" s="13"/>
     </row>
     <row r="47" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
@@ -1179,7 +1182,7 @@
       <c r="B47" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C47" s="12"/>
+      <c r="C47" s="13"/>
     </row>
     <row r="48" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
@@ -1188,7 +1191,7 @@
       <c r="B48" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C48" s="12"/>
+      <c r="C48" s="13"/>
     </row>
     <row r="49" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
@@ -1197,7 +1200,7 @@
       <c r="B49" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C49" s="12"/>
+      <c r="C49" s="13"/>
     </row>
     <row r="50" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
@@ -1206,7 +1209,7 @@
       <c r="B50" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C50" s="12"/>
+      <c r="C50" s="13"/>
     </row>
     <row r="51" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
@@ -1215,7 +1218,7 @@
       <c r="B51" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C51" s="12"/>
+      <c r="C51" s="13"/>
     </row>
     <row r="52" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
@@ -1224,7 +1227,7 @@
       <c r="B52" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C52" s="12"/>
+      <c r="C52" s="13"/>
     </row>
     <row r="53" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
@@ -1282,7 +1285,7 @@
       <c r="H57" s="1">
         <v>137.5</v>
       </c>
-      <c r="I57" s="13">
+      <c r="I57" s="12">
         <v>43852</v>
       </c>
       <c r="J57" s="1">
@@ -1316,7 +1319,7 @@
         <v>1</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E59" s="1">
         <v>7</v>
@@ -1330,7 +1333,7 @@
         <v>2</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E60" s="1">
         <v>6</v>
@@ -1384,7 +1387,7 @@
         <v>1</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E66" s="1">
         <v>8</v>
@@ -1398,7 +1401,7 @@
         <v>2</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E67" s="1">
         <v>4</v>
@@ -1427,6 +1430,12 @@
       <c r="B70" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="C70" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E70" s="1">
+        <v>4</v>
+      </c>
     </row>
     <row r="71" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A71" s="2">
@@ -1437,11 +1446,11 @@
       </c>
       <c r="F71" s="1">
         <f>SUM(E58:E71)</f>
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="G71" s="1">
         <f>F71*20</f>
-        <v>640</v>
+        <v>720</v>
       </c>
       <c r="I71" s="7"/>
     </row>

</xml_diff>

<commit_message>
redefined graphs and data converted
</commit_message>
<xml_diff>
--- a/_NCSA Time sheet.xlsx
+++ b/_NCSA Time sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/snehgajiwala/Desktop/NCSA_genomics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB785CC1-C152-7844-B7E5-EE5F0D95E55F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60539CDE-7EB4-8A48-ACDC-72C66B3ECCA9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16460" xr2:uid="{AD204971-E0E7-594B-AE4B-D8231DE2D531}"/>
   </bookViews>
@@ -23,7 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="32">
   <si>
     <t>Monday</t>
   </si>
@@ -124,6 +126,9 @@
   </si>
   <si>
     <t>9:00 to 15:00 =&gt;  Studying and implementing the 'mice' library</t>
+  </si>
+  <si>
+    <t>9:00 to 16:00 =&gt; Meeting with Justina; Reworking some of the plots to fit appropriate ranges; Reworking imputations by applying conversions; Designing boxplots instead of average line graphs</t>
   </si>
 </sst>
 </file>
@@ -555,10 +560,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22F60381-B2D6-6E48-8C0F-6899A86E0E4E}">
-  <dimension ref="A2:K77"/>
+  <dimension ref="A2:K87"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C70" sqref="C70"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="C73" sqref="C73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1454,12 +1459,18 @@
       </c>
       <c r="I71" s="7"/>
     </row>
-    <row r="72" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A72" s="2">
         <v>43857</v>
       </c>
       <c r="B72" s="3" t="s">
         <v>0</v>
+      </c>
+      <c r="C72" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E72" s="1">
+        <v>7</v>
       </c>
     </row>
     <row r="73" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -1500,6 +1511,94 @@
       </c>
       <c r="B77" s="3" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A78" s="2">
+        <v>43863</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A79" s="2">
+        <v>43864</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A80" s="2">
+        <v>43865</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A81" s="2">
+        <v>43866</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A82" s="2">
+        <v>43867</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A83" s="2">
+        <v>43868</v>
+      </c>
+      <c r="B83" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A84" s="2">
+        <v>43869</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A85" s="2">
+        <v>43870</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F85" s="1">
+        <f>SUM(E72:E84)</f>
+        <v>7</v>
+      </c>
+      <c r="G85" s="1">
+        <f>F85*20</f>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A86" s="2">
+        <v>43871</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A87" s="2">
+        <v>43872</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
plots, plots, plots (also bug fixing)
</commit_message>
<xml_diff>
--- a/_NCSA Time sheet.xlsx
+++ b/_NCSA Time sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/snehgajiwala/Desktop/NCSA_genomics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF4794AE-9A6B-A345-855C-5CFAEFA563B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03AF484B-9C61-554C-83A7-876046CE1DFD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16460" xr2:uid="{AD204971-E0E7-594B-AE4B-D8231DE2D531}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="35">
   <si>
     <t>Monday</t>
   </si>
@@ -95,9 +95,6 @@
     <t>Meeting</t>
   </si>
   <si>
-    <t>on Dec 11</t>
-  </si>
-  <si>
     <t>https://journals.sagepub.com/doi/full/10.1177/1932296817710478</t>
   </si>
   <si>
@@ -131,13 +128,16 @@
     <t>9:00 to 16:00 =&gt; Meeting with Justina; Reworking some of the plots to fit appropriate ranges; Reworking imputations by applying conversions; Designing boxplots instead of average line graphs</t>
   </si>
   <si>
-    <t>9:00 to 17:00 =&gt;</t>
-  </si>
-  <si>
-    <t>9:00 to 13:00 =&gt;</t>
-  </si>
-  <si>
     <t>9:00 to 13:00 =&gt; Adding multiple gaps of 5,10,…,100 to check the effects</t>
+  </si>
+  <si>
+    <t>9:00 to 17:00 =&gt; Meeting with Justina; Correcting error metrics =&gt; working out the bugs</t>
+  </si>
+  <si>
+    <t>9:00 to 17:00 =&gt; Working on the bugs; meeting with sophia; reworking the plots</t>
+  </si>
+  <si>
+    <t>9:00 to 13:00 =&gt; Researching on consensus approaches</t>
   </si>
 </sst>
 </file>
@@ -213,7 +213,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -250,6 +250,9 @@
     </xf>
     <xf numFmtId="16" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -569,10 +572,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22F60381-B2D6-6E48-8C0F-6899A86E0E4E}">
-  <dimension ref="A2:K96"/>
+  <dimension ref="A2:K109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="F85" sqref="F85"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="D81" sqref="D81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -589,7 +592,7 @@
     <col min="11" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>43787</v>
       </c>
@@ -598,7 +601,7 @@
       </c>
       <c r="C2" s="4"/>
     </row>
-    <row r="3" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>43788</v>
       </c>
@@ -612,7 +615,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>43789</v>
       </c>
@@ -621,7 +624,7 @@
       </c>
       <c r="C4" s="4"/>
     </row>
-    <row r="5" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>43790</v>
       </c>
@@ -630,7 +633,7 @@
       </c>
       <c r="C5" s="4"/>
     </row>
-    <row r="6" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>43791</v>
       </c>
@@ -644,7 +647,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>43792</v>
       </c>
@@ -653,7 +656,7 @@
       </c>
       <c r="C7" s="4"/>
     </row>
-    <row r="8" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>43793</v>
       </c>
@@ -662,7 +665,7 @@
       </c>
       <c r="C8" s="4"/>
     </row>
-    <row r="9" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>43794</v>
       </c>
@@ -676,7 +679,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>43795</v>
       </c>
@@ -690,7 +693,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>43796</v>
       </c>
@@ -718,11 +721,16 @@
       <c r="I11" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="J11" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="J11" s="1">
+        <f>H11/G11</f>
+        <v>0.92849999999999999</v>
+      </c>
+      <c r="K11" s="1">
+        <f>(1-J11)*100</f>
+        <v>7.15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>43797</v>
       </c>
@@ -731,7 +739,7 @@
       </c>
       <c r="C12" s="4"/>
     </row>
-    <row r="13" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>43798</v>
       </c>
@@ -740,7 +748,7 @@
       </c>
       <c r="C13" s="4"/>
     </row>
-    <row r="14" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>43799</v>
       </c>
@@ -756,7 +764,7 @@
       <c r="I14" s="11"/>
       <c r="J14" s="11"/>
     </row>
-    <row r="15" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>43800</v>
       </c>
@@ -772,7 +780,7 @@
       <c r="I15" s="11"/>
       <c r="J15" s="11"/>
     </row>
-    <row r="16" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>43801</v>
       </c>
@@ -948,7 +956,7 @@
         <v>4</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E27" s="1">
         <v>2</v>
@@ -1005,10 +1013,10 @@
         <v>0</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E30" s="1">
         <v>8</v>
@@ -1035,7 +1043,7 @@
       <c r="B32" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C32" s="13" t="s">
+      <c r="C32" s="14" t="s">
         <v>14</v>
       </c>
       <c r="D32" s="10"/>
@@ -1048,9 +1056,9 @@
       <c r="B33" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C33" s="13"/>
-      <c r="D33" s="10"/>
-      <c r="E33" s="10"/>
+      <c r="C33" s="14"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="11"/>
     </row>
     <row r="34" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
@@ -1059,7 +1067,7 @@
       <c r="B34" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C34" s="13"/>
+      <c r="C34" s="14"/>
     </row>
     <row r="35" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
@@ -1068,7 +1076,7 @@
       <c r="B35" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C35" s="13"/>
+      <c r="C35" s="14"/>
     </row>
     <row r="36" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
@@ -1077,7 +1085,7 @@
       <c r="B36" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C36" s="13"/>
+      <c r="C36" s="14"/>
     </row>
     <row r="37" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
@@ -1086,7 +1094,7 @@
       <c r="B37" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C37" s="13"/>
+      <c r="C37" s="14"/>
     </row>
     <row r="38" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
@@ -1095,7 +1103,7 @@
       <c r="B38" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C38" s="13"/>
+      <c r="C38" s="14"/>
     </row>
     <row r="39" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
@@ -1104,7 +1112,7 @@
       <c r="B39" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C39" s="13"/>
+      <c r="C39" s="14"/>
     </row>
     <row r="40" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
@@ -1113,7 +1121,7 @@
       <c r="B40" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C40" s="13"/>
+      <c r="C40" s="14"/>
     </row>
     <row r="41" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
@@ -1122,7 +1130,7 @@
       <c r="B41" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C41" s="13"/>
+      <c r="C41" s="14"/>
     </row>
     <row r="42" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
@@ -1131,7 +1139,7 @@
       <c r="B42" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C42" s="13"/>
+      <c r="C42" s="14"/>
     </row>
     <row r="43" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
@@ -1140,7 +1148,7 @@
       <c r="B43" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C43" s="13"/>
+      <c r="C43" s="14"/>
       <c r="F43" s="1">
         <f>SUM(E30:E41)</f>
         <v>9</v>
@@ -1169,7 +1177,7 @@
       <c r="B44" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C44" s="13"/>
+      <c r="C44" s="14"/>
     </row>
     <row r="45" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
@@ -1178,7 +1186,7 @@
       <c r="B45" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C45" s="13"/>
+      <c r="C45" s="14"/>
     </row>
     <row r="46" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
@@ -1187,7 +1195,7 @@
       <c r="B46" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C46" s="13"/>
+      <c r="C46" s="14"/>
     </row>
     <row r="47" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
@@ -1196,7 +1204,7 @@
       <c r="B47" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C47" s="13"/>
+      <c r="C47" s="14"/>
     </row>
     <row r="48" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
@@ -1205,7 +1213,7 @@
       <c r="B48" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C48" s="13"/>
+      <c r="C48" s="14"/>
     </row>
     <row r="49" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
@@ -1214,7 +1222,7 @@
       <c r="B49" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C49" s="13"/>
+      <c r="C49" s="14"/>
     </row>
     <row r="50" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
@@ -1223,7 +1231,7 @@
       <c r="B50" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C50" s="13"/>
+      <c r="C50" s="14"/>
     </row>
     <row r="51" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
@@ -1232,7 +1240,7 @@
       <c r="B51" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C51" s="13"/>
+      <c r="C51" s="14"/>
     </row>
     <row r="52" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
@@ -1241,7 +1249,7 @@
       <c r="B52" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C52" s="13"/>
+      <c r="C52" s="14"/>
     </row>
     <row r="53" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
@@ -1268,7 +1276,7 @@
         <v>4</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E55" s="1">
         <v>7</v>
@@ -1289,7 +1297,10 @@
       <c r="B57" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F57" s="1">
+      <c r="C57" s="13"/>
+      <c r="D57" s="10"/>
+      <c r="E57" s="10"/>
+      <c r="F57" s="11">
         <v>7</v>
       </c>
       <c r="G57" s="1">
@@ -1319,7 +1330,7 @@
         <v>0</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E58" s="1">
         <v>7</v>
@@ -1333,7 +1344,7 @@
         <v>1</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E59" s="1">
         <v>7</v>
@@ -1347,7 +1358,7 @@
         <v>2</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E60" s="1">
         <v>6</v>
@@ -1401,7 +1412,7 @@
         <v>1</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E66" s="1">
         <v>8</v>
@@ -1415,7 +1426,7 @@
         <v>2</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E67" s="1">
         <v>4</v>
@@ -1445,7 +1456,7 @@
         <v>5</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E70" s="1">
         <v>4</v>
@@ -1458,6 +1469,9 @@
       <c r="B71" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="C71" s="13"/>
+      <c r="D71" s="10"/>
+      <c r="E71" s="10"/>
       <c r="F71" s="1">
         <f>SUM(E58:E71)</f>
         <v>36</v>
@@ -1466,6 +1480,10 @@
         <f>F71*20</f>
         <v>720</v>
       </c>
+      <c r="H71" s="1">
+        <f>G71*0.9285</f>
+        <v>668.52</v>
+      </c>
       <c r="I71" s="7"/>
     </row>
     <row r="72" spans="1:9" ht="51" x14ac:dyDescent="0.2">
@@ -1476,7 +1494,7 @@
         <v>0</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E72" s="1">
         <v>7</v>
@@ -1490,7 +1508,7 @@
         <v>1</v>
       </c>
       <c r="C73" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E73" s="1">
         <v>4</v>
@@ -1558,7 +1576,7 @@
         <v>1</v>
       </c>
       <c r="C80" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E80" s="1">
         <v>8</v>
@@ -1572,7 +1590,7 @@
         <v>2</v>
       </c>
       <c r="C81" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E81" s="1">
         <v>4</v>
@@ -1609,6 +1627,9 @@
       <c r="B85" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="C85" s="13"/>
+      <c r="D85" s="10"/>
+      <c r="E85" s="10"/>
       <c r="F85" s="1">
         <f>SUM(E72:E84)</f>
         <v>31</v>
@@ -1617,6 +1638,10 @@
         <f>F85*20</f>
         <v>620</v>
       </c>
+      <c r="H85" s="1">
+        <f>G85*0.9285</f>
+        <v>575.66999999999996</v>
+      </c>
       <c r="I85" s="7"/>
     </row>
     <row r="86" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -1705,6 +1730,113 @@
       </c>
       <c r="B96" s="3" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A97" s="2">
+        <v>43882</v>
+      </c>
+      <c r="B97" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A98" s="2">
+        <v>43883</v>
+      </c>
+      <c r="B98" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A99" s="2">
+        <v>43884</v>
+      </c>
+      <c r="B99" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C99" s="13"/>
+      <c r="D99" s="10"/>
+      <c r="E99" s="10"/>
+    </row>
+    <row r="100" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A100" s="2">
+        <v>43885</v>
+      </c>
+      <c r="B100" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A101" s="2">
+        <v>43886</v>
+      </c>
+      <c r="B101" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A102" s="2">
+        <v>43887</v>
+      </c>
+      <c r="B102" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A103" s="2">
+        <v>43888</v>
+      </c>
+      <c r="B103" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A104" s="2">
+        <v>43889</v>
+      </c>
+      <c r="B104" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A105" s="2">
+        <v>43890</v>
+      </c>
+      <c r="B105" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A106" s="2">
+        <v>43891</v>
+      </c>
+      <c r="B106" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A107" s="2">
+        <v>43892</v>
+      </c>
+      <c r="B107" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A108" s="2">
+        <v>43893</v>
+      </c>
+      <c r="B108" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A109" s="2">
+        <v>43894</v>
+      </c>
+      <c r="B109" s="3" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
working on sophia's data
</commit_message>
<xml_diff>
--- a/_NCSA Time sheet.xlsx
+++ b/_NCSA Time sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/snehgajiwala/Desktop/NCSA_genomics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03AF484B-9C61-554C-83A7-876046CE1DFD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E50128AC-9853-CA45-885B-DACCB2666F53}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16460" xr2:uid="{AD204971-E0E7-594B-AE4B-D8231DE2D531}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="38">
   <si>
     <t>Monday</t>
   </si>
@@ -138,13 +138,22 @@
   </si>
   <si>
     <t>9:00 to 13:00 =&gt; Researching on consensus approaches</t>
+  </si>
+  <si>
+    <t>11:00 to 17:00 =&gt; Working in data provided by Sophia; Group Meeting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9:00 to 16:00 =&gt; Meeting with Justina; </t>
+  </si>
+  <si>
+    <t>9:00 to 16:00 =&gt;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -173,8 +182,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -199,6 +216,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -213,7 +236,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -253,6 +276,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -572,10 +604,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22F60381-B2D6-6E48-8C0F-6899A86E0E4E}">
-  <dimension ref="A2:K109"/>
+  <dimension ref="A2:N135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="D81" sqref="D81"/>
+    <sheetView tabSelected="1" topLeftCell="A78" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C132" sqref="C132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -589,10 +621,11 @@
     <col min="8" max="8" width="13.83203125" style="1" customWidth="1"/>
     <col min="9" max="9" width="13" style="1" customWidth="1"/>
     <col min="10" max="10" width="18.6640625" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="10.83203125" style="1"/>
+    <col min="11" max="11" width="10.83203125" style="16"/>
+    <col min="12" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>43787</v>
       </c>
@@ -601,7 +634,7 @@
       </c>
       <c r="C2" s="4"/>
     </row>
-    <row r="3" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>43788</v>
       </c>
@@ -615,7 +648,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>43789</v>
       </c>
@@ -624,7 +657,7 @@
       </c>
       <c r="C4" s="4"/>
     </row>
-    <row r="5" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>43790</v>
       </c>
@@ -633,7 +666,7 @@
       </c>
       <c r="C5" s="4"/>
     </row>
-    <row r="6" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>43791</v>
       </c>
@@ -647,7 +680,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>43792</v>
       </c>
@@ -656,7 +689,7 @@
       </c>
       <c r="C7" s="4"/>
     </row>
-    <row r="8" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>43793</v>
       </c>
@@ -665,7 +698,7 @@
       </c>
       <c r="C8" s="4"/>
     </row>
-    <row r="9" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>43794</v>
       </c>
@@ -679,7 +712,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>43795</v>
       </c>
@@ -693,7 +726,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>43796</v>
       </c>
@@ -725,12 +758,16 @@
         <f>H11/G11</f>
         <v>0.92849999999999999</v>
       </c>
-      <c r="K11" s="1">
+      <c r="K11" s="16">
         <f>(1-J11)*100</f>
         <v>7.15</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L11" s="1">
+        <f>G11-H11</f>
+        <v>32.175000000000011</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>43797</v>
       </c>
@@ -739,7 +776,7 @@
       </c>
       <c r="C12" s="4"/>
     </row>
-    <row r="13" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>43798</v>
       </c>
@@ -748,7 +785,7 @@
       </c>
       <c r="C13" s="4"/>
     </row>
-    <row r="14" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>43799</v>
       </c>
@@ -764,7 +801,7 @@
       <c r="I14" s="11"/>
       <c r="J14" s="11"/>
     </row>
-    <row r="15" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>43800</v>
       </c>
@@ -780,7 +817,7 @@
       <c r="I15" s="11"/>
       <c r="J15" s="11"/>
     </row>
-    <row r="16" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>43801</v>
       </c>
@@ -799,7 +836,7 @@
       <c r="I16" s="11"/>
       <c r="J16" s="11"/>
     </row>
-    <row r="17" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>43802</v>
       </c>
@@ -813,7 +850,7 @@
       <c r="I17" s="11"/>
       <c r="J17" s="11"/>
     </row>
-    <row r="18" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>43803</v>
       </c>
@@ -832,7 +869,7 @@
       <c r="I18" s="11"/>
       <c r="J18" s="11"/>
     </row>
-    <row r="19" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>43804</v>
       </c>
@@ -851,7 +888,7 @@
       <c r="I19" s="11"/>
       <c r="J19" s="11"/>
     </row>
-    <row r="20" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>43805</v>
       </c>
@@ -865,7 +902,7 @@
       <c r="I20" s="11"/>
       <c r="J20" s="11"/>
     </row>
-    <row r="21" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>43806</v>
       </c>
@@ -881,7 +918,7 @@
       <c r="I21" s="11"/>
       <c r="J21" s="11"/>
     </row>
-    <row r="22" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>43807</v>
       </c>
@@ -897,7 +934,7 @@
       <c r="I22" s="11"/>
       <c r="J22" s="11"/>
     </row>
-    <row r="23" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>43808</v>
       </c>
@@ -911,7 +948,7 @@
       <c r="I23" s="11"/>
       <c r="J23" s="11"/>
     </row>
-    <row r="24" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>43809</v>
       </c>
@@ -920,7 +957,7 @@
       </c>
       <c r="C24" s="4"/>
     </row>
-    <row r="25" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>43810</v>
       </c>
@@ -934,7 +971,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>43811</v>
       </c>
@@ -948,7 +985,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>43812</v>
       </c>
@@ -962,7 +999,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>43813</v>
       </c>
@@ -973,7 +1010,7 @@
       <c r="D28" s="10"/>
       <c r="E28" s="10"/>
     </row>
-    <row r="29" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>43814</v>
       </c>
@@ -1000,12 +1037,16 @@
         <f>H29/G29</f>
         <v>0.9285000000000001</v>
       </c>
-      <c r="K29" s="1">
+      <c r="K29" s="16">
         <f>(1-J29)*100</f>
         <v>7.1499999999999897</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+      <c r="L29" s="1">
+        <f>G29-H29</f>
+        <v>40.039999999999964</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>43815</v>
       </c>
@@ -1022,7 +1063,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>43816</v>
       </c>
@@ -1036,119 +1077,119 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>43817</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C32" s="14" t="s">
+      <c r="C32" s="17" t="s">
         <v>14</v>
       </c>
       <c r="D32" s="10"/>
       <c r="E32" s="10"/>
     </row>
-    <row r="33" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>43818</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C33" s="14"/>
+      <c r="C33" s="17"/>
       <c r="D33" s="11"/>
       <c r="E33" s="11"/>
     </row>
-    <row r="34" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>43819</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C34" s="14"/>
-    </row>
-    <row r="35" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="C34" s="17"/>
+    </row>
+    <row r="35" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>43820</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C35" s="14"/>
-    </row>
-    <row r="36" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="C35" s="17"/>
+    </row>
+    <row r="36" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>43821</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C36" s="14"/>
-    </row>
-    <row r="37" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="C36" s="17"/>
+    </row>
+    <row r="37" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>43822</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C37" s="14"/>
-    </row>
-    <row r="38" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="C37" s="17"/>
+    </row>
+    <row r="38" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>43823</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C38" s="14"/>
-    </row>
-    <row r="39" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="C38" s="17"/>
+    </row>
+    <row r="39" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>43824</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C39" s="14"/>
-    </row>
-    <row r="40" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="C39" s="17"/>
+    </row>
+    <row r="40" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>43825</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C40" s="14"/>
-    </row>
-    <row r="41" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="C40" s="17"/>
+    </row>
+    <row r="41" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>43826</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C41" s="14"/>
-    </row>
-    <row r="42" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="C41" s="17"/>
+    </row>
+    <row r="42" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>43827</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C42" s="14"/>
-    </row>
-    <row r="43" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="C42" s="17"/>
+    </row>
+    <row r="43" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>43828</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C43" s="14"/>
+      <c r="C43" s="17"/>
       <c r="F43" s="1">
         <f>SUM(E30:E41)</f>
         <v>9</v>
@@ -1165,93 +1206,97 @@
         <f>H43/G43</f>
         <v>0.97222222222222221</v>
       </c>
-      <c r="K43" s="1">
+      <c r="K43" s="16">
         <f>(1-J43)*100</f>
         <v>2.777777777777779</v>
       </c>
-    </row>
-    <row r="44" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L43" s="1">
+        <f>G43-H43</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>43829</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C44" s="14"/>
-    </row>
-    <row r="45" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="C44" s="17"/>
+    </row>
+    <row r="45" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
         <v>43830</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C45" s="14"/>
-    </row>
-    <row r="46" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="C45" s="17"/>
+    </row>
+    <row r="46" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>43831</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C46" s="14"/>
-    </row>
-    <row r="47" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="C46" s="17"/>
+    </row>
+    <row r="47" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
         <v>43832</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C47" s="14"/>
-    </row>
-    <row r="48" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="C47" s="17"/>
+    </row>
+    <row r="48" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
         <v>43833</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C48" s="14"/>
-    </row>
-    <row r="49" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="C48" s="17"/>
+    </row>
+    <row r="49" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
         <v>43834</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C49" s="14"/>
-    </row>
-    <row r="50" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="C49" s="17"/>
+    </row>
+    <row r="50" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
         <v>43835</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C50" s="14"/>
-    </row>
-    <row r="51" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="C50" s="17"/>
+    </row>
+    <row r="51" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
         <v>43836</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C51" s="14"/>
-    </row>
-    <row r="52" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="C51" s="17"/>
+    </row>
+    <row r="52" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
         <v>43837</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C52" s="14"/>
-    </row>
-    <row r="53" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="C52" s="17"/>
+    </row>
+    <row r="53" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
         <v>43838</v>
       </c>
@@ -1260,7 +1305,7 @@
       </c>
       <c r="C53" s="4"/>
     </row>
-    <row r="54" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
         <v>43839</v>
       </c>
@@ -1268,7 +1313,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
         <v>43840</v>
       </c>
@@ -1282,7 +1327,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="56" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
         <v>43841</v>
       </c>
@@ -1290,7 +1335,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="57" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
         <v>43842</v>
       </c>
@@ -1317,12 +1362,16 @@
         <f>H57/G57</f>
         <v>0.9821428571428571</v>
       </c>
-      <c r="K57" s="1">
+      <c r="K57" s="16">
         <f>(1-J57)*100</f>
         <v>1.7857142857142905</v>
       </c>
-    </row>
-    <row r="58" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="L57" s="1">
+        <f>G57-H57</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
         <v>43843</v>
       </c>
@@ -1336,7 +1385,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="59" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
         <v>43844</v>
       </c>
@@ -1350,7 +1399,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
         <v>43845</v>
       </c>
@@ -1364,7 +1413,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="61" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A61" s="2">
         <v>43846</v>
       </c>
@@ -1372,7 +1421,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="62" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A62" s="2">
         <v>43847</v>
       </c>
@@ -1380,7 +1429,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="63" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A63" s="2">
         <v>43848</v>
       </c>
@@ -1388,7 +1437,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="64" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A64" s="2">
         <v>43849</v>
       </c>
@@ -1396,7 +1445,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="65" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A65" s="2">
         <v>43850</v>
       </c>
@@ -1404,7 +1453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A66" s="2">
         <v>43851</v>
       </c>
@@ -1418,7 +1467,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="67" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A67" s="2">
         <v>43852</v>
       </c>
@@ -1432,7 +1481,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="68" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A68" s="2">
         <v>43853</v>
       </c>
@@ -1440,7 +1489,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="69" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A69" s="2">
         <v>43854</v>
       </c>
@@ -1448,7 +1497,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="70" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A70" s="2">
         <v>43855</v>
       </c>
@@ -1462,7 +1511,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="71" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A71" s="2">
         <v>43856</v>
       </c>
@@ -1481,12 +1530,27 @@
         <v>720</v>
       </c>
       <c r="H71" s="1">
-        <f>G71*0.9285</f>
-        <v>668.52</v>
-      </c>
-      <c r="I71" s="7"/>
-    </row>
-    <row r="72" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+        <v>647.37</v>
+      </c>
+      <c r="I71" s="6"/>
+      <c r="J71" s="1">
+        <f>H71/G71</f>
+        <v>0.89912499999999995</v>
+      </c>
+      <c r="K71" s="16">
+        <f>(1-J71)*100</f>
+        <v>10.087500000000006</v>
+      </c>
+      <c r="L71" s="1">
+        <f>G71-H71</f>
+        <v>72.63</v>
+      </c>
+      <c r="N71" s="1">
+        <f>SUM(L1:L71)</f>
+        <v>152.34499999999997</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A72" s="2">
         <v>43857</v>
       </c>
@@ -1500,7 +1564,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="73" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A73" s="2">
         <v>43858</v>
       </c>
@@ -1514,7 +1578,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="74" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A74" s="2">
         <v>43859</v>
       </c>
@@ -1522,7 +1586,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A75" s="2">
         <v>43860</v>
       </c>
@@ -1530,7 +1594,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="76" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A76" s="2">
         <v>43861</v>
       </c>
@@ -1538,7 +1602,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="77" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A77" s="2">
         <v>43862</v>
       </c>
@@ -1546,7 +1610,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="78" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A78" s="2">
         <v>43863</v>
       </c>
@@ -1554,7 +1618,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="79" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A79" s="2">
         <v>43864</v>
       </c>
@@ -1568,7 +1632,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="80" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A80" s="2">
         <v>43865</v>
       </c>
@@ -1595,6 +1659,7 @@
       <c r="E81" s="1">
         <v>4</v>
       </c>
+      <c r="I81" s="14"/>
     </row>
     <row r="82" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A82" s="2">
@@ -1638,10 +1703,6 @@
         <f>F85*20</f>
         <v>620</v>
       </c>
-      <c r="H85" s="1">
-        <f>G85*0.9285</f>
-        <v>575.66999999999996</v>
-      </c>
       <c r="I85" s="7"/>
     </row>
     <row r="86" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -1651,6 +1712,12 @@
       <c r="B86" s="3" t="s">
         <v>0</v>
       </c>
+      <c r="C86" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E86" s="1">
+        <v>6</v>
+      </c>
     </row>
     <row r="87" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A87" s="2">
@@ -1659,6 +1726,12 @@
       <c r="B87" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="C87" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E87" s="1">
+        <v>7</v>
+      </c>
     </row>
     <row r="88" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A88" s="2">
@@ -1667,6 +1740,12 @@
       <c r="B88" s="3" t="s">
         <v>2</v>
       </c>
+      <c r="C88" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E88" s="1">
+        <v>7</v>
+      </c>
     </row>
     <row r="89" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A89" s="2">
@@ -1723,6 +1802,7 @@
       <c r="B95" s="3" t="s">
         <v>2</v>
       </c>
+      <c r="I95" s="14"/>
     </row>
     <row r="96" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A96" s="2">
@@ -1732,7 +1812,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="97" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A97" s="2">
         <v>43882</v>
       </c>
@@ -1740,7 +1820,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="98" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A98" s="2">
         <v>43883</v>
       </c>
@@ -1748,7 +1828,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="99" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A99" s="2">
         <v>43884</v>
       </c>
@@ -1758,8 +1838,17 @@
       <c r="C99" s="13"/>
       <c r="D99" s="10"/>
       <c r="E99" s="10"/>
-    </row>
-    <row r="100" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="F99" s="1">
+        <f>SUM(E86:E98)</f>
+        <v>20</v>
+      </c>
+      <c r="G99" s="1">
+        <f>F99*20</f>
+        <v>400</v>
+      </c>
+      <c r="I99" s="7"/>
+    </row>
+    <row r="100" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A100" s="2">
         <v>43885</v>
       </c>
@@ -1767,7 +1856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A101" s="2">
         <v>43886</v>
       </c>
@@ -1775,7 +1864,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A102" s="2">
         <v>43887</v>
       </c>
@@ -1783,7 +1872,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="103" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A103" s="2">
         <v>43888</v>
       </c>
@@ -1791,7 +1880,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="104" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A104" s="2">
         <v>43889</v>
       </c>
@@ -1799,7 +1888,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="105" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A105" s="2">
         <v>43890</v>
       </c>
@@ -1807,7 +1896,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="106" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A106" s="2">
         <v>43891</v>
       </c>
@@ -1815,7 +1904,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="107" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A107" s="2">
         <v>43892</v>
       </c>
@@ -1823,7 +1912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A108" s="2">
         <v>43893</v>
       </c>
@@ -1831,12 +1920,233 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A109" s="2">
         <v>43894</v>
       </c>
       <c r="B109" s="3" t="s">
         <v>2</v>
+      </c>
+      <c r="I109" s="14"/>
+    </row>
+    <row r="110" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A110" s="2">
+        <v>43895</v>
+      </c>
+      <c r="B110" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A111" s="2">
+        <v>43896</v>
+      </c>
+      <c r="B111" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A112" s="2">
+        <v>43897</v>
+      </c>
+      <c r="B112" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A113" s="2">
+        <v>43898</v>
+      </c>
+      <c r="B113" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C113" s="13"/>
+      <c r="D113" s="10"/>
+      <c r="E113" s="10"/>
+      <c r="F113" s="1">
+        <f>SUM(E100:E112)</f>
+        <v>0</v>
+      </c>
+      <c r="G113" s="1">
+        <f>F113*20</f>
+        <v>0</v>
+      </c>
+      <c r="I113" s="15"/>
+    </row>
+    <row r="114" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A114" s="2">
+        <v>43899</v>
+      </c>
+      <c r="B114" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A115" s="2">
+        <v>43900</v>
+      </c>
+      <c r="B115" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A116" s="2">
+        <v>43901</v>
+      </c>
+      <c r="B116" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A117" s="2">
+        <v>43902</v>
+      </c>
+      <c r="B117" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A118" s="2">
+        <v>43903</v>
+      </c>
+      <c r="B118" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A119" s="2">
+        <v>43904</v>
+      </c>
+      <c r="B119" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A120" s="2">
+        <v>43905</v>
+      </c>
+      <c r="B120" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A121" s="2">
+        <v>43906</v>
+      </c>
+      <c r="B121" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A122" s="2">
+        <v>43907</v>
+      </c>
+      <c r="B122" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A123" s="2">
+        <v>43908</v>
+      </c>
+      <c r="B123" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A124" s="2">
+        <v>43909</v>
+      </c>
+      <c r="B124" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A125" s="2">
+        <v>43910</v>
+      </c>
+      <c r="B125" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A126" s="2">
+        <v>43911</v>
+      </c>
+      <c r="B126" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A127" s="2">
+        <v>43912</v>
+      </c>
+      <c r="B127" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A128" s="2">
+        <v>43913</v>
+      </c>
+      <c r="B128" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A129" s="2">
+        <v>43914</v>
+      </c>
+      <c r="B129" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A130" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B130" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A131" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B131" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A132" s="2">
+        <v>43917</v>
+      </c>
+      <c r="B132" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A133" s="2">
+        <v>43918</v>
+      </c>
+      <c r="B133" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A134" s="2">
+        <v>43919</v>
+      </c>
+      <c r="B134" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A135" s="2">
+        <v>43920</v>
+      </c>
+      <c r="B135" s="3" t="s">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
started building tensorflow model
</commit_message>
<xml_diff>
--- a/_NCSA Time sheet.xlsx
+++ b/_NCSA Time sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/snehgajiwala/Desktop/NCSA_genomics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E50128AC-9853-CA45-885B-DACCB2666F53}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D353D76-31C0-2F43-9051-F3EBE17DE097}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16460" xr2:uid="{AD204971-E0E7-594B-AE4B-D8231DE2D531}"/>
   </bookViews>
@@ -143,10 +143,10 @@
     <t>11:00 to 17:00 =&gt; Working in data provided by Sophia; Group Meeting</t>
   </si>
   <si>
-    <t xml:space="preserve">9:00 to 16:00 =&gt; Meeting with Justina; </t>
-  </si>
-  <si>
     <t>9:00 to 16:00 =&gt;</t>
+  </si>
+  <si>
+    <t>9:00 to 16:00 =&gt; Meeting with Justina; Meeting with sophia; Starting to work on the daya in python; Building a simple predictive model using Tensorflow</t>
   </si>
 </sst>
 </file>
@@ -606,8 +606,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22F60381-B2D6-6E48-8C0F-6899A86E0E4E}">
   <dimension ref="A2:N135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A78" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C132" sqref="C132"/>
+    <sheetView tabSelected="1" topLeftCell="A80" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C88" sqref="C88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1719,15 +1719,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="87" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A87" s="2">
         <v>43872</v>
       </c>
       <c r="B87" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C87" s="5" t="s">
-        <v>36</v>
+      <c r="C87" s="4" t="s">
+        <v>37</v>
       </c>
       <c r="E87" s="1">
         <v>7</v>
@@ -1741,7 +1741,7 @@
         <v>2</v>
       </c>
       <c r="C88" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E88" s="1">
         <v>7</v>

</xml_diff>